<commit_message>
added munit > 90%
</commit_message>
<xml_diff>
--- a/API Design Review Checklist.xlsx
+++ b/API Design Review Checklist.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Anypoint\studio-workspace\fakestore-cart-prc-api\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LewisCao\AnypointStudio\studio-workspace\fakestore-product-prc-api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC0AD84D-F5EC-4C0C-8E59-C4BCDDD61405}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84FCE409-483D-4886-A7D4-3C0AE6109C3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" activeTab="1" xr2:uid="{4CC6B8E9-9D48-48E9-9569-A1A540D0340B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" activeTab="3" xr2:uid="{4CC6B8E9-9D48-48E9-9569-A1A540D0340B}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="8" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="52">
   <si>
     <t>API is protected by at least basic auth or clientid and clientsecret</t>
   </si>
@@ -781,8 +781,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5256589-1EC7-4A8D-B58F-CAB97A906BDF}">
   <dimension ref="A1:B38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -922,7 +922,9 @@
       <c r="A19" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B19" s="2"/>
+      <c r="B19" s="4" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
@@ -1071,7 +1073,7 @@
   <dimension ref="A1:B38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A38"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1211,7 +1213,9 @@
       <c r="A19" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B19" s="2"/>
+      <c r="B19" s="4" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
@@ -1359,8 +1363,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2888403C-429B-4C25-98F8-DABCF40C815D}">
   <dimension ref="A1:B38"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1500,7 +1504,9 @@
       <c r="A19" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B19" s="2"/>
+      <c r="B19" s="4" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">

</xml_diff>